<commit_message>
adding a qst to the dataset
</commit_message>
<xml_diff>
--- a/data/Q&A_COVID-19(1).xlsx
+++ b/data/Q&A_COVID-19(1).xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="30" windowWidth="20730" windowHeight="10050"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="283">
   <si>
     <t>question</t>
   </si>
@@ -1140,6 +1140,13 @@
   </si>
   <si>
     <t>i'm developped by a team of two enginners students IDALI LAHCEN Abdessalam And ECCHARAY Mohammed from Ensah School</t>
+  </si>
+  <si>
+    <t>are lahcen abdessalam And eccharay Mohammed your developers?</t>
+  </si>
+  <si>
+    <t>Yes of course, They did a great job. I am not a perfect bot but a great one. 
+If you want to test me, try asking me what ever you want about covid-19. Or simplly start a regular discussion with me.</t>
   </si>
 </sst>
 </file>
@@ -1518,10 +1525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B142"/>
+  <dimension ref="A1:B143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B128" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="B137" sqref="B137"/>
+    <sheetView tabSelected="1" topLeftCell="B139" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="B143" sqref="B143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2664,6 +2671,14 @@
       </c>
       <c r="B142" s="2" t="s">
         <v>276</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A143" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>282</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixing typo in data
</commit_message>
<xml_diff>
--- a/data/Q&A_COVID-19(1).xlsx
+++ b/data/Q&A_COVID-19(1).xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="30" windowWidth="20730" windowHeight="10050"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="287">
   <si>
     <t>question</t>
   </si>
@@ -1147,6 +1147,18 @@
   </si>
   <si>
     <t>you know python, flutter, AI, deep learning i'm a mixt of those things what about you, tell me about your self what do you love ?</t>
+  </si>
+  <si>
+    <t>who is idali lahcen abdessalam ?</t>
+  </si>
+  <si>
+    <t>he is a student engineer at ENSAH, one of my founders you can contact him on sibawayh.idali@gmail.com</t>
+  </si>
+  <si>
+    <t>he is a student engineer at ENSAH, one of my founders you can contact him on echcharaymoh@gmail.com</t>
+  </si>
+  <si>
+    <t>who is mohamed ech-charay</t>
   </si>
 </sst>
 </file>
@@ -1525,10 +1537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B143"/>
+  <dimension ref="A1:B145"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A129" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="A143" sqref="A143"/>
+      <selection activeCell="A145" sqref="A145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2679,6 +2691,22 @@
       </c>
       <c r="B143" s="2" t="s">
         <v>275</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>285</v>
       </c>
     </row>
   </sheetData>

</xml_diff>